<commit_message>
create plots for individual lexical items
</commit_message>
<xml_diff>
--- a/stats/data/stem_data_simplified.xlsx
+++ b/stats/data/stem_data_simplified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7cf2c9d3dc7fdc6/Dissertation/stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{2753A57D-B923-404A-8773-F4C4678CE3B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F1E69DF8-822C-40AC-8C33-EC40E23FC78E}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{2753A57D-B923-404A-8773-F4C4678CE3B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1998E168-60B1-4221-88D1-3479C0FA29DE}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{6192CA4F-71F8-4549-AC06-999AD8CF57D5}"/>
   </bookViews>
@@ -6170,7 +6170,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B7E85-307C-429B-BC44-F5509FAE785C}">
-  <dimension ref="A1:AE403"/>
+  <dimension ref="A1:F403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -16023,7 +16023,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16050,790 +16050,790 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>606</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>607</v>
+        <v>113</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>273</v>
       </c>
       <c r="D2">
-        <v>0.47812574707147998</v>
+        <v>32.632082237628502</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.120323985162579</v>
       </c>
       <c r="F2">
-        <v>0.89110686110447002</v>
+        <v>0.26074710212888602</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>870</v>
+        <v>525</v>
       </c>
       <c r="B3" t="s">
-        <v>575</v>
+        <v>526</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>139</v>
       </c>
       <c r="D3">
-        <v>0.47812574707147998</v>
+        <v>16.614869710733899</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3.8838193102460401E-2</v>
       </c>
       <c r="F3">
-        <v>0.89110686110447002</v>
+        <v>0.18991481450268899</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>593</v>
+        <v>429</v>
       </c>
       <c r="B4" t="s">
-        <v>594</v>
+        <v>105</v>
       </c>
       <c r="C4">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="D4">
-        <v>4.5421945971790603</v>
+        <v>9.6820463781974695</v>
       </c>
       <c r="E4">
-        <v>0.113097986133275</v>
+        <v>0.106413199946327</v>
       </c>
       <c r="F4">
-        <v>0.57861393862375299</v>
+        <v>0.34060113982816997</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>599</v>
+        <v>446</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>447</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>0.47812574707147998</v>
+        <v>7.1718862060722</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.47574252126094302</v>
       </c>
       <c r="F5">
-        <v>0.75866602916567105</v>
+        <v>0.29442983504661702</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>869</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D6">
-        <v>1.3148458044465701</v>
+        <v>6.2156347119292397</v>
       </c>
       <c r="E6">
-        <v>0.27729172565378901</v>
+        <v>0.606472774141669</v>
       </c>
       <c r="F6">
-        <v>0.72842457566340002</v>
+        <v>0.39342393203258602</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>593</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>594</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D7">
-        <v>1.9125029882859199</v>
+        <v>4.5421945971790603</v>
       </c>
       <c r="E7">
-        <v>0.21280633861277301</v>
+        <v>0.113097986133275</v>
       </c>
       <c r="F7">
-        <v>0.46705414774085602</v>
+        <v>0.57861393862375299</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>612</v>
+        <v>841</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>581</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>0.59765718383934996</v>
+        <v>4.1836002868754498</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.41702080323255097</v>
       </c>
       <c r="F8">
-        <v>0.92039206311259902</v>
+        <v>0.54851610259212502</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>856</v>
+        <v>685</v>
       </c>
       <c r="B9" t="s">
-        <v>857</v>
+        <v>83</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>0.95625149414295996</v>
+        <v>4.0640688501075797</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.651860046831921</v>
       </c>
       <c r="F9">
-        <v>0.827038010996892</v>
+        <v>0.42442800691876098</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>850</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>0.71718862060722</v>
+        <v>3.8250059765718398</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.72101362658379198</v>
+        <v>0.35583761654315099</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>855</v>
+        <v>255</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>2.51016017212527</v>
+        <v>3.4664116662682298</v>
       </c>
       <c r="E11">
-        <v>0.76090298016176205</v>
+        <v>0.13653126326509599</v>
       </c>
       <c r="F11">
-        <v>0.50634655009505602</v>
+        <v>0.42052395987041102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>868</v>
+        <v>416</v>
       </c>
       <c r="B12" t="s">
-        <v>845</v>
+        <v>417</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>0.59765718383934996</v>
+        <v>3.4664116662682298</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.22842890703676899</v>
       </c>
       <c r="F12">
-        <v>0.97824527850824805</v>
+        <v>0.49086614952146201</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>839</v>
+        <v>811</v>
       </c>
       <c r="B13" t="s">
-        <v>840</v>
+        <v>777</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D13">
-        <v>0.83672005737509003</v>
+        <v>3.3468802295003601</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0.64965335883337305</v>
+        <v>0.31232710631467497</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>755</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>756</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D14">
-        <v>1.43437724121444</v>
+        <v>3.3468802295003601</v>
       </c>
       <c r="E14">
-        <v>0.26108936338578798</v>
+        <v>0.14024611344719401</v>
       </c>
       <c r="F14">
-        <v>0.59705952665551099</v>
+        <v>0.44753423721867402</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>841</v>
+        <v>862</v>
       </c>
       <c r="B15" t="s">
-        <v>581</v>
+        <v>863</v>
       </c>
       <c r="C15">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>4.1836002868754498</v>
+        <v>2.9882859191967501</v>
       </c>
       <c r="E15">
-        <v>0.41702080323255097</v>
+        <v>0.40020477099739299</v>
       </c>
       <c r="F15">
-        <v>0.54851610259212502</v>
+        <v>0.48901267033229701</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>262</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>0.47812574707147998</v>
+        <v>2.7492230456610098</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.84150131484580504</v>
+        <v>0.79180741926430998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>855</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D17">
-        <v>0.47812574707147998</v>
+        <v>2.51016017212527</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.76090298016176205</v>
       </c>
       <c r="F17">
-        <v>0.91238345684915101</v>
+        <v>0.50634655009505602</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
+        <v>62</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>0.47812574707147998</v>
+        <v>2.51016017212527</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.96748744919913898</v>
+        <v>0.53237594344455397</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>239</v>
+        <v>750</v>
       </c>
       <c r="B19" t="s">
-        <v>240</v>
+        <v>751</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>0.71718862060722</v>
+        <v>2.51016017212527</v>
       </c>
       <c r="E19">
-        <v>0.78969008214284797</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.77348792732488603</v>
+        <v>0.54202952995685505</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>803</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>804</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D20">
-        <v>0.59765718383934996</v>
+        <v>2.3906287353573998</v>
       </c>
       <c r="E20">
-        <v>0.61260161928934398</v>
+        <v>0.91971732357509295</v>
       </c>
       <c r="F20">
-        <v>0.69878077934496796</v>
+        <v>0.55571360267750403</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C21">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D21">
-        <v>6.2156347119292397</v>
+        <v>2.2710972985895301</v>
       </c>
       <c r="E21">
-        <v>0.606472774141669</v>
+        <v>0.187684092704995</v>
       </c>
       <c r="F21">
-        <v>0.39342393203258602</v>
+        <v>0.431521068988512</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>871</v>
+        <v>626</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>627</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D22">
-        <v>0.71718862060722</v>
+        <v>2.2710972985895301</v>
       </c>
       <c r="E22">
-        <v>0.57938016428569505</v>
+        <v>0.83505545115915503</v>
       </c>
       <c r="F22">
-        <v>0.62777910590485297</v>
+        <v>0.32214980434591101</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>719</v>
       </c>
       <c r="B23" t="s">
-        <v>202</v>
+        <v>720</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>0.71718862060722</v>
+        <v>2.2710972985895301</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.82058331341142698</v>
+        <v>0.49426878216339298</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D24">
-        <v>1.07578293091083</v>
+        <v>1.9125029882859199</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.21280633861277301</v>
       </c>
       <c r="F24">
-        <v>0.57709777671527596</v>
+        <v>0.46705414774085602</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="B25" t="s">
-        <v>198</v>
+        <v>315</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>0.59765718383934996</v>
+        <v>1.9125029882859199</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.21280633861277301</v>
       </c>
       <c r="F25">
-        <v>0.867320105187665</v>
+        <v>0.47625806837198198</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>205</v>
+        <v>864</v>
       </c>
       <c r="B26" t="s">
-        <v>206</v>
+        <v>863</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D26">
-        <v>0.95625149414295996</v>
+        <v>1.79297155151805</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.45548591500359498</v>
       </c>
       <c r="F26">
-        <v>0.64284006693760498</v>
+        <v>0.38528169575264998</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>874</v>
       </c>
       <c r="B27" t="s">
-        <v>209</v>
+        <v>278</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D27">
-        <v>1.07578293091083</v>
+        <v>1.79297155151805</v>
       </c>
       <c r="E27">
-        <v>0.62529937420430104</v>
+        <v>0.22294491816723899</v>
       </c>
       <c r="F27">
-        <v>0.74324647382261499</v>
+        <v>0.83065582914973302</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>667</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>668</v>
       </c>
       <c r="C28">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>2.2710972985895301</v>
+        <v>1.6734401147501801</v>
       </c>
       <c r="E28">
-        <v>0.187684092704995</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0.431521068988512</v>
+        <v>0.69338478877087595</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>224</v>
+        <v>383</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>384</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D29">
-        <v>0.47812574707147998</v>
+        <v>1.5539086779823099</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.56183767112112704</v>
       </c>
       <c r="F29">
-        <v>0.95995696868276403</v>
+        <v>0.82374629912282304</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>878</v>
       </c>
       <c r="B30" t="s">
-        <v>234</v>
+        <v>433</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D30">
-        <v>1.1953143676786999</v>
+        <v>1.5539086779823099</v>
       </c>
       <c r="E30">
-        <v>0.29590327428938501</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0.51379392780301203</v>
+        <v>0.90102797035620397</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>862</v>
+        <v>879</v>
       </c>
       <c r="B31" t="s">
-        <v>863</v>
+        <v>475</v>
       </c>
       <c r="C31">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>2.9882859191967501</v>
+        <v>1.5539086779823099</v>
       </c>
       <c r="E31">
-        <v>0.40020477099739299</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>0.48901267033229701</v>
+        <v>0.46861840048548098</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>864</v>
+        <v>787</v>
       </c>
       <c r="B32" t="s">
-        <v>863</v>
+        <v>788</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D32">
-        <v>1.79297155151805</v>
+        <v>1.5539086779823099</v>
       </c>
       <c r="E32">
-        <v>0.45548591500359498</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0.38528169575264998</v>
+        <v>0.61988083635226898</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>255</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="C33">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>3.4664116662682298</v>
+        <v>1.43437724121444</v>
       </c>
       <c r="E33">
-        <v>0.13653126326509599</v>
+        <v>0.26108936338578798</v>
       </c>
       <c r="F33">
-        <v>0.42052395987041102</v>
+        <v>0.59705952665551099</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>257</v>
+        <v>332</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>333</v>
       </c>
       <c r="C34">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D34">
-        <v>3.8250059765718398</v>
+        <v>1.43437724121444</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.35583761654315099</v>
+        <v>0.85249820702844803</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>860</v>
+        <v>672</v>
       </c>
       <c r="B35" t="s">
-        <v>861</v>
+        <v>673</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D35">
-        <v>0.83672005737509003</v>
+        <v>1.43437724121444</v>
       </c>
       <c r="E35">
-        <v>0.37330396038588698</v>
+        <v>0.41011848630651798</v>
       </c>
       <c r="F35">
-        <v>0.85859431030361</v>
+        <v>0.46171009642202598</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>303</v>
+        <v>869</v>
       </c>
       <c r="B36" t="s">
-        <v>304</v>
+        <v>162</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D36">
-        <v>0.59765718383934996</v>
+        <v>1.3148458044465701</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.27729172565378901</v>
       </c>
       <c r="F36">
-        <v>0.88560841501314802</v>
+        <v>0.72842457566340002</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>261</v>
+        <v>359</v>
       </c>
       <c r="B37" t="s">
-        <v>262</v>
+        <v>124</v>
       </c>
       <c r="C37">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>2.7492230456610098</v>
+        <v>1.3148458044465701</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0.79180741926430998</v>
+        <v>0.76320822376285002</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>873</v>
+        <v>737</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>738</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>0.47812574707147998</v>
+        <v>1.3148458044465701</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0.80910829548171204</v>
+        <v>0.659031143372525</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>874</v>
+        <v>233</v>
       </c>
       <c r="B39" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="C39">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>1.79297155151805</v>
+        <v>1.1953143676786999</v>
       </c>
       <c r="E39">
-        <v>0.22294491816723899</v>
+        <v>0.29590327428938501</v>
       </c>
       <c r="F39">
-        <v>0.83065582914973302</v>
+        <v>0.51379392780301203</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>872</v>
+        <v>289</v>
       </c>
       <c r="B40" t="s">
-        <v>308</v>
+        <v>32</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D40">
-        <v>0.71718862060722</v>
+        <v>1.1953143676786999</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>0.29590327428938501</v>
       </c>
       <c r="F40">
-        <v>0.560841501314846</v>
+        <v>0.62691847956012403</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>289</v>
+        <v>362</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C41">
         <v>10</v>
@@ -16842,338 +16842,338 @@
         <v>1.1953143676786999</v>
       </c>
       <c r="E41">
-        <v>0.29590327428938501</v>
+        <v>0.55603264987638901</v>
       </c>
       <c r="F41">
-        <v>0.62691847956012403</v>
+        <v>0.872818551278986</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>296</v>
+        <v>877</v>
       </c>
       <c r="B42" t="s">
-        <v>297</v>
+        <v>398</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D42">
-        <v>0.95625149414295996</v>
+        <v>1.1953143676786999</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.61260161928934398</v>
       </c>
       <c r="F42">
-        <v>0.89935453024145395</v>
+        <v>0.61037532871145095</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>650</v>
+        <v>191</v>
       </c>
       <c r="B43" t="s">
-        <v>651</v>
+        <v>192</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D43">
-        <v>0.83672005737509003</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0.82966770260578504</v>
+        <v>0.57709777671527596</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>615</v>
+        <v>208</v>
       </c>
       <c r="B44" t="s">
-        <v>616</v>
+        <v>209</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>0.59765718383934996</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>0.62529937420430104</v>
       </c>
       <c r="F44">
-        <v>0.84293569208701902</v>
+        <v>0.74324647382261499</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="B45" t="s">
-        <v>618</v>
+        <v>352</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D45">
-        <v>0.47812574707147998</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>0.60218081026566805</v>
       </c>
       <c r="F45">
-        <v>0.71001673440114799</v>
+        <v>0.72089409514702396</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>619</v>
+        <v>403</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>404</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D46">
-        <v>0.83672005737509003</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0.90867798230934704</v>
+        <v>0.73409567827449695</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>648</v>
+        <v>499</v>
       </c>
       <c r="B47" t="s">
-        <v>649</v>
+        <v>500</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D47">
-        <v>0.71718862060722</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.31752065714277999</v>
       </c>
       <c r="F47">
-        <v>0.77265120726751102</v>
+        <v>0.65269476983557795</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>626</v>
+        <v>493</v>
       </c>
       <c r="B48" t="s">
-        <v>627</v>
+        <v>23</v>
       </c>
       <c r="C48">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D48">
-        <v>2.2710972985895301</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E48">
-        <v>0.83505545115915503</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>0.32214980434591101</v>
+        <v>0.65902993598427495</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>664</v>
+        <v>783</v>
       </c>
       <c r="B49" t="s">
-        <v>663</v>
+        <v>784</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D49">
-        <v>0.59765718383934996</v>
+        <v>1.07578293091083</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.62529937420430104</v>
       </c>
       <c r="F49">
-        <v>0.61343533349270896</v>
+        <v>0.60136265837915404</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>642</v>
+        <v>856</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>857</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50">
-        <v>0.83672005737509003</v>
+        <v>0.95625149414295996</v>
       </c>
       <c r="E50">
-        <v>0.544568447628201</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>0.63076739182404995</v>
+        <v>0.827038010996892</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>325</v>
+        <v>205</v>
       </c>
       <c r="B51" t="s">
-        <v>326</v>
+        <v>206</v>
       </c>
       <c r="C51">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D51">
-        <v>0.71718862060722</v>
+        <v>0.95625149414295996</v>
       </c>
       <c r="E51">
-        <v>0.41011848630651798</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>0.70846282572316499</v>
+        <v>0.64284006693760498</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
       <c r="B52" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="C52">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>1.43437724121444</v>
+        <v>0.95625149414295996</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0.85249820702844803</v>
+        <v>0.89935453024145395</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>314</v>
+        <v>425</v>
       </c>
       <c r="B53" t="s">
-        <v>315</v>
+        <v>426</v>
       </c>
       <c r="C53">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D53">
-        <v>1.9125029882859199</v>
+        <v>0.95625149414295996</v>
       </c>
       <c r="E53">
-        <v>0.21280633861277301</v>
+        <v>0.60218081026566805</v>
       </c>
       <c r="F53">
-        <v>0.47625806837198198</v>
+        <v>0.48075543868037302</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>311</v>
+        <v>471</v>
       </c>
       <c r="B54" t="s">
-        <v>312</v>
+        <v>126</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D54">
-        <v>0.71718862060722</v>
+        <v>0.95625149414295996</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0.66435572555582101</v>
+        <v>0.78460435094429803</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>875</v>
+        <v>839</v>
       </c>
       <c r="B55" t="s">
-        <v>352</v>
+        <v>840</v>
       </c>
       <c r="C55">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D55">
-        <v>1.07578293091083</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E55">
-        <v>0.60218081026566805</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>0.72089409514702396</v>
+        <v>0.64965335883337305</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>876</v>
+        <v>860</v>
       </c>
       <c r="B56" t="s">
-        <v>350</v>
+        <v>861</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D56">
-        <v>0.71718862060722</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E56">
-        <v>0.61260161928934398</v>
+        <v>0.37330396038588698</v>
       </c>
       <c r="F56">
-        <v>0.87485058570403995</v>
+        <v>0.85859431030361</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>359</v>
+        <v>650</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>651</v>
       </c>
       <c r="C57">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D57">
-        <v>1.3148458044465701</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0.76320822376285002</v>
+        <v>0.82966770260578504</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>394</v>
+        <v>619</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -17185,535 +17185,535 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0.51111642361941201</v>
+        <v>0.90867798230934704</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>362</v>
+        <v>642</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D59">
-        <v>1.1953143676786999</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E59">
-        <v>0.55603264987638901</v>
+        <v>0.544568447628201</v>
       </c>
       <c r="F59">
-        <v>0.872818551278986</v>
+        <v>0.63076739182404995</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="B60" t="s">
-        <v>368</v>
+        <v>30</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D60">
-        <v>0.71718862060722</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0.79285202008128097</v>
+        <v>0.51111642361941201</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>373</v>
+        <v>771</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>772</v>
       </c>
       <c r="C61">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D61">
-        <v>2.51016017212527</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0.53237594344455397</v>
+        <v>0.775639493186708</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>383</v>
+        <v>766</v>
       </c>
       <c r="B62" t="s">
-        <v>384</v>
+        <v>734</v>
       </c>
       <c r="C62">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D62">
-        <v>1.5539086779823099</v>
+        <v>0.83672005737509003</v>
       </c>
       <c r="E62">
-        <v>0.56183767112112704</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0.82374629912282304</v>
+        <v>0.58881185751852805</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>877</v>
+        <v>850</v>
       </c>
       <c r="B63" t="s">
-        <v>398</v>
+        <v>53</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63">
-        <v>1.1953143676786999</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E63">
-        <v>0.61260161928934398</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>0.61037532871145095</v>
+        <v>0.72101362658379198</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>403</v>
+        <v>239</v>
       </c>
       <c r="B64" t="s">
-        <v>404</v>
+        <v>240</v>
       </c>
       <c r="C64">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D64">
-        <v>1.07578293091083</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>0.78969008214284797</v>
       </c>
       <c r="F64">
-        <v>0.73409567827449695</v>
+        <v>0.77348792732488603</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>416</v>
+        <v>871</v>
       </c>
       <c r="B65" t="s">
-        <v>417</v>
+        <v>232</v>
       </c>
       <c r="C65">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D65">
-        <v>3.4664116662682298</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E65">
-        <v>0.22842890703676899</v>
+        <v>0.57938016428569505</v>
       </c>
       <c r="F65">
-        <v>0.49086614952146201</v>
+        <v>0.62777910590485297</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>408</v>
+        <v>201</v>
       </c>
       <c r="B66" t="s">
-        <v>409</v>
+        <v>202</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D66">
-        <v>0.59765718383934996</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.67069089170451801</v>
+        <v>0.82058331341142698</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>420</v>
+        <v>872</v>
       </c>
       <c r="B67" t="s">
-        <v>421</v>
+        <v>308</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D67">
-        <v>0.59765718383934996</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0.566339947406168</v>
+        <v>0.560841501314846</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>429</v>
+        <v>648</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>649</v>
       </c>
       <c r="C68">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="D68">
-        <v>9.6820463781974695</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E68">
-        <v>0.106413199946327</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>0.34060113982816997</v>
+        <v>0.77265120726751102</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>425</v>
+        <v>325</v>
       </c>
       <c r="B69" t="s">
-        <v>426</v>
+        <v>326</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D69">
-        <v>0.95625149414295996</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E69">
-        <v>0.60218081026566805</v>
+        <v>0.41011848630651798</v>
       </c>
       <c r="F69">
-        <v>0.48075543868037302</v>
+        <v>0.70846282572316499</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>878</v>
+        <v>311</v>
       </c>
       <c r="B70" t="s">
-        <v>433</v>
+        <v>312</v>
       </c>
       <c r="C70">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>1.5539086779823099</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0.90102797035620397</v>
+        <v>0.66435572555582101</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>446</v>
+        <v>876</v>
       </c>
       <c r="B71" t="s">
-        <v>447</v>
+        <v>350</v>
       </c>
       <c r="C71">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D71">
-        <v>7.1718862060722</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E71">
-        <v>0.47574252126094302</v>
+        <v>0.61260161928934398</v>
       </c>
       <c r="F71">
-        <v>0.29442983504661702</v>
+        <v>0.87485058570403995</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>464</v>
+        <v>367</v>
       </c>
       <c r="B72" t="s">
-        <v>465</v>
+        <v>368</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D72">
-        <v>0.47812574707147998</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.94262491035142204</v>
+        <v>0.79285202008128097</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>471</v>
+        <v>665</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>666</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D73">
-        <v>0.95625149414295996</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0.78460435094429803</v>
+        <v>0.61439158498685198</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>879</v>
+        <v>700</v>
       </c>
       <c r="B74" t="s">
-        <v>475</v>
+        <v>701</v>
       </c>
       <c r="C74">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D74">
-        <v>1.5539086779823099</v>
+        <v>0.71718862060722</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>0.63092975357145797</v>
       </c>
       <c r="F74">
-        <v>0.46861840048548098</v>
+        <v>0.68814248147262702</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>499</v>
+        <v>612</v>
       </c>
       <c r="B75" t="s">
-        <v>500</v>
+        <v>90</v>
       </c>
       <c r="C75">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D75">
-        <v>1.07578293091083</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E75">
-        <v>0.31752065714277999</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>0.65269476983557795</v>
+        <v>0.92039206311259902</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>493</v>
+        <v>868</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>845</v>
       </c>
       <c r="C76">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D76">
-        <v>1.07578293091083</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0.65902993598427495</v>
+        <v>0.97824527850824805</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>486</v>
+        <v>182</v>
       </c>
       <c r="B77" t="s">
-        <v>487</v>
+        <v>26</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D77">
-        <v>0.47812574707147998</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>0.61260161928934398</v>
       </c>
       <c r="F77">
-        <v>0.74970117140808001</v>
+        <v>0.69878077934496796</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>509</v>
+        <v>197</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="C78">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="D78">
-        <v>32.632082237628502</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E78">
-        <v>0.120323985162579</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>0.26074710212888602</v>
+        <v>0.867320105187665</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>880</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s">
-        <v>513</v>
+        <v>304</v>
       </c>
       <c r="C79">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D79">
-        <v>0.47812574707147998</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79">
-        <v>0.92911785799665303</v>
+        <v>0.88560841501314802</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>525</v>
+        <v>615</v>
       </c>
       <c r="B80" t="s">
-        <v>526</v>
+        <v>616</v>
       </c>
       <c r="C80">
-        <v>139</v>
+        <v>5</v>
       </c>
       <c r="D80">
-        <v>16.614869710733899</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E80">
-        <v>3.8838193102460401E-2</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>0.18991481450268899</v>
+        <v>0.84293569208701902</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B81" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C81">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D81">
-        <v>0.71718862060722</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0.61439158498685198</v>
+        <v>0.61343533349270896</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>667</v>
+        <v>408</v>
       </c>
       <c r="B82" t="s">
-        <v>668</v>
+        <v>409</v>
       </c>
       <c r="C82">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D82">
-        <v>1.6734401147501801</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0.69338478877087595</v>
+        <v>0.67069089170451801</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>700</v>
+        <v>420</v>
       </c>
       <c r="B83" t="s">
-        <v>701</v>
+        <v>421</v>
       </c>
       <c r="C83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83">
-        <v>0.71718862060722</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E83">
-        <v>0.63092975357145797</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>0.68814248147262702</v>
+        <v>0.566339947406168</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>672</v>
+        <v>805</v>
       </c>
       <c r="B84" t="s">
-        <v>673</v>
+        <v>806</v>
       </c>
       <c r="C84">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D84">
-        <v>1.43437724121444</v>
+        <v>0.59765718383934996</v>
       </c>
       <c r="E84">
-        <v>0.41011848630651798</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>0.46171009642202598</v>
+        <v>0.63411427205354998</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>866</v>
+        <v>606</v>
       </c>
       <c r="B85" t="s">
-        <v>679</v>
+        <v>607</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -17725,15 +17725,15 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0.64044943820224698</v>
+        <v>0.89110686110447002</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>684</v>
+        <v>870</v>
       </c>
       <c r="B86" t="s">
-        <v>96</v>
+        <v>575</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -17745,35 +17745,35 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0.67750418360028697</v>
+        <v>0.89110686110447002</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>685</v>
+        <v>599</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="C87">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D87">
-        <v>4.0640688501075797</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E87">
-        <v>0.651860046831921</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>0.42442800691876098</v>
+        <v>0.75866602916567105</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>819</v>
+        <v>177</v>
       </c>
       <c r="B88" t="s">
-        <v>820</v>
+        <v>36</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -17782,38 +17782,38 @@
         <v>0.47812574707147998</v>
       </c>
       <c r="E88">
-        <v>0.51185950714291495</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>0.75484102318909896</v>
+        <v>0.84150131484580504</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>719</v>
+        <v>235</v>
       </c>
       <c r="B89" t="s">
-        <v>720</v>
+        <v>236</v>
       </c>
       <c r="C89">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D89">
-        <v>2.2710972985895301</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0.49426878216339298</v>
+        <v>0.91238345684915101</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>730</v>
+        <v>237</v>
       </c>
       <c r="B90" t="s">
-        <v>731</v>
+        <v>238</v>
       </c>
       <c r="C90">
         <v>4</v>
@@ -17825,75 +17825,75 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0.78819029404733498</v>
+        <v>0.96748744919913898</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>803</v>
+        <v>224</v>
       </c>
       <c r="B91" t="s">
-        <v>804</v>
+        <v>225</v>
       </c>
       <c r="C91">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D91">
-        <v>2.3906287353573998</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E91">
-        <v>0.91971732357509295</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>0.55571360267750403</v>
+        <v>0.95995696868276403</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>805</v>
+        <v>873</v>
       </c>
       <c r="B92" t="s">
-        <v>806</v>
+        <v>281</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D92">
-        <v>0.59765718383934996</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0.63411427205354998</v>
+        <v>0.80910829548171204</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>737</v>
+        <v>617</v>
       </c>
       <c r="B93" t="s">
-        <v>738</v>
+        <v>618</v>
       </c>
       <c r="C93">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D93">
-        <v>1.3148458044465701</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <v>0.659031143372525</v>
+        <v>0.71001673440114799</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>867</v>
+        <v>464</v>
       </c>
       <c r="B94" t="s">
-        <v>796</v>
+        <v>465</v>
       </c>
       <c r="C94">
         <v>4</v>
@@ -17905,152 +17905,152 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0.95661008845326301</v>
+        <v>0.94262491035142204</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>811</v>
+        <v>486</v>
       </c>
       <c r="B95" t="s">
-        <v>777</v>
+        <v>487</v>
       </c>
       <c r="C95">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D95">
-        <v>3.3468802295003601</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>0.31232710631467497</v>
+        <v>0.74970117140808001</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>771</v>
+        <v>880</v>
       </c>
       <c r="B96" t="s">
-        <v>772</v>
+        <v>513</v>
       </c>
       <c r="C96">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D96">
-        <v>0.83672005737509003</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>0.775639493186708</v>
+        <v>0.92911785799665303</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>750</v>
+        <v>866</v>
       </c>
       <c r="B97" t="s">
-        <v>751</v>
+        <v>679</v>
       </c>
       <c r="C97">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D97">
-        <v>2.51016017212527</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>0.54202952995685505</v>
+        <v>0.64044943820224698</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>755</v>
+        <v>684</v>
       </c>
       <c r="B98" t="s">
-        <v>756</v>
+        <v>96</v>
       </c>
       <c r="C98">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D98">
-        <v>3.3468802295003601</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E98">
-        <v>0.14024611344719401</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>0.44753423721867402</v>
+        <v>0.67750418360028697</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>783</v>
+        <v>819</v>
       </c>
       <c r="B99" t="s">
-        <v>784</v>
+        <v>820</v>
       </c>
       <c r="C99">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D99">
-        <v>1.07578293091083</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E99">
-        <v>0.62529937420430104</v>
+        <v>0.51185950714291495</v>
       </c>
       <c r="F99">
-        <v>0.60136265837915404</v>
+        <v>0.75484102318909896</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>787</v>
+        <v>730</v>
       </c>
       <c r="B100" t="s">
-        <v>788</v>
+        <v>731</v>
       </c>
       <c r="C100">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D100">
-        <v>1.5539086779823099</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0.61988083635226898</v>
+        <v>0.78819029404733498</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>766</v>
+        <v>867</v>
       </c>
       <c r="B101" t="s">
-        <v>734</v>
+        <v>796</v>
       </c>
       <c r="C101">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D101">
-        <v>0.83672005737509003</v>
+        <v>0.47812574707147998</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101">
-        <v>0.58881185751852805</v>
+        <v>0.95661008845326301</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F102">
-    <sortCondition ref="A1:A102"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
+    <sortCondition descending="1" ref="C1:C101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>